<commit_message>
kmeans clustering with optimize per cost of amount
</commit_message>
<xml_diff>
--- a/tutorial/output/eblocks-plate-upload-template-96-filled.xlsx
+++ b/tutorial/output/eblocks-plate-upload-template-96-filled.xlsx
@@ -458,12 +458,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>V1108I_Block-6</t>
+          <t>T224W_Block-1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>cgagatgctgggactgtacgtctcggggcatcccctcaacggtgtggcacacttgctggctgcccaggtcgacaccgcgatcccagcgatcctcgacggcgatgtccccaacgatgcccaagtgcgggtgggcggcatcctggcgtcggtgaaccggagggtcaacaaaaacggaatgccatgggcttcagcgcaattggaggatctcacgggcggcatcgaggtgatgttcttcccgcacacctactccagctatggtgccgacatcgtcgacgatgccgtcgtgctggtcaacgccaaggtggcggtccgtgacgaccgcatcgcattgatcgccaatgacctcacagtgcccgacttttccaacgccgagatcgagcggccgctggcggtcagcttgcccacccggcagtgcacctttgacaaggtgagtgcgctcaaacaggtgttggcgcgccaccccggcacct</t>
+          <t>gatgcccgcggtggggatgaccgaccacggaaacatgttcggtgccagcgagttctacaactccgcgaccaaggccgggatcaagccgatcatcggcgtggaggcatacatcgcgccgggctcgcggttcgacacccggcgcatcctgtggggtgaccccagccaaaaggccgacgacgtctccggcagcggctcctacacgcacctgacgatgatggccgagaacgccaccggtctgcgcaacctgttcaagctgtcctcgcatgcttccttcgagggccagctgagcaagtggtcgcgcatggacgccgagctcatcgccgaacacgccgagggcatcatcatcaccaccggatgcccgtcgggggaggtgcagacccgcctgcggctcggccaggatcgggaggcgctcgaagccgcggcgaagtggcgggagatcgtcggaccggacaactacttccttgagctgatggaccacgggctgaccatcgaacgccgggtccgtgacggtctgctcgagatcggacgcgcgctcaacattccgcctcttgcctggaatgactgccactacgtgacccgcgacgccgcccacaaccatgaggctttgttgtgtgtgcagaccggcaagaccctctcggatccgaatcgcttcaagttcgacggtgacggctactacctgaagtcggccgccgagatgcgccagatctgggacgacgaagtgccgggcgcgtgtgactccaccttgttgatcgccgaacgggtgcagtcctacgccgacgtgtggacaccgcgcgaccggatgcccgtgtttccggtgcccgatgggcatgaccaggcgtcctggctgcgtcacgaggtggacgccgggcttcgcc</t>
         </is>
       </c>
     </row>
@@ -475,12 +475,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>G1041T_Block-6</t>
+          <t>E184E_Block-1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>cgagatgctgggactgtacgtctcggggcatcccctcaacggtgtggcacacttgctggctgcccaggtcgacaccgcgatcccagcgatcctcgacggcgatgtccccaacgatgcccaagtgcgggtgggcggcatcctggcgtcggtgaaccggagggtcaacaaaaacaccatgccatgggcttcagcgcaattggaggatctcacgggcggcatcgaggtgatgttcttcccgcacacctactccagctatggtgccgacatcgtcgacgatgccgtcgtgctggtcaacgccaaggtggcggtccgtgacgaccgcatcgcattgatcgccaatgacctcacagtgcccgacttttccaacgccgaggtggagcggccgctggcggtcagcttgcccacccggcagtgcacctttgacaaggtgagtgcgctcaaacaggtgttggcgcgccaccccggcacct</t>
+          <t>gatgcccgcggtggggatgaccgaccacggaaacatgttcggtgccagcgagttctacaactccgcgaccaaggccgggatcaagccgatcatcggcgtggaggcatacatcgcgccgggctcgcggttcgacacccggcgcatcctgtggggtgaccccagccaaaaggccgacgacgtctccggcagcggctcctacacgcacctgacgatgatggccgagaacgccaccggtctgcgcaacctgttcaagctgtcctcgcatgcttccttcgagggccagctgagcaagtggtcgcgcatggacgccgagctcatcgccgaacacgccgagggcatcatcatcaccaccggatgcccgtcgggggaggtgcagacccgcctgcggctcggccaggatcgggaggcgctcgaagccgcggcgaagtggcgggagatcgtcggaccggacaactacttccttgagctgatggaccacgggctgaccatcgaacgccgggtccgtgacggtctgctcgagatcggacgcgcgctcaacattccgcctcttgccaccaatgactgccactacgtgacccgcgacgccgcccacaaccatgaggctttgttgtgtgtgcagaccggcaagaccctctcggatccgaatcgcttcaagttcgacggtgacggctactacctgaagtcggccgccgagatgcgccagatctgggacgacgaagtgccgggcgcgtgtgactccaccttgttgatcgccgaacgggtgcagtcctacgccgacgtgtggacaccgcgcgaccggatgcccgtgtttccggtgcccgatgggcatgaccaggcgtcctggctgcgtcacgaggtggacgccgggcttcgcc</t>
         </is>
       </c>
     </row>
@@ -492,12 +492,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Y827R_Block-4</t>
+          <t>Y859T_Block-3</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>gccgttcgctgactacgcgttcaacaagtcacatgccgccggctacggcatggtgtcctactggacggcctacctcaaggccaactatcccgccgagtacatggccggtctgttgacgtcggtcggcgacgataaagacaaggccgcggttcgcctggccgactgccgcaagctcggcatcaccgtgctcccgcccgacgtcaacgaatctggcttgaacttcgcatcggtcggccaagacatccgctacgggctgggcgcggtgcgcaacgttggcgctaatgtcgtgggctcgttgctccaaacccgcaacgacaagggcaagttcaccgacttttcggactacctgaacaagatcgacatctcggcgtgcaacaagaaggtgaccgaatcgctgatcaaggcgggtgcgttcgactcgctggggcatgcccgcaagggtcttttcctggtgcacagcgatgcgg</t>
+          <t>cgacattctacgcaaggccatgggcaagaagaaacgcgaggtgctggagaaggagttcgagggcttctccgatggcatgcaggccaacgggttctctccggcggccatcaaggcgctgtgggacaccatcctgccgttcgctgactacgcgttcaacaagtcacatgccgccggctacggcatggtgtcctactggacggcctacctcaaggccaactatcccgccgagtacatggccggtctgttgacgtcggtcggcgacgataaagacaaggccgcggtttatctggccgactgccgcaagctcggcatcaccgtgctcccgcccgacgtcaacgaatctggcttgaacttcgcatcggtcggccaagacatccgcaccgggctgggcgcggtgcgcaacgttggcgctaatgtcgtgggctcgttgctccaaacccgcaacgacaagggcaagttcaccgacttttcggactacctgaacaagatcgacatctcggcgtgcaacaagaaggtgaccgaatcgctgatcaaggcgggtgcgttcgactcgctggggcatgcccgcaagggtcttttcctggtgcacagcgatgcggtggactcggtgctgggcaccaagaaggccgaggcactggggcagttcgatctcttcggcagcaatgatgatgggaccggcaccgcagatcccgtgttcaccatcaaggtgcccgatgatgagtgggaggacaaacacaaactcgccctagagcgcgagatgctgggactgtacgtctcggggcatcccctcaacggtgtggcacacttgctggctgcccaggtcgacaccgcgatcccagcgatcctcgacggcgatgtccccaacgatgcccaagtgcgggtgggcggcatcctggcgtcggtgaaccggagggtcaacaaaaacggaatgccatgggcttcagcgcaattggaggatctcacgggcggcatcgaggtgatgttcttcccgcacacctactccagctatggtgccgacatcgtcgacgatgccgtcgtgctggtcaacgccaaggtggcggtccgtgacgaccgcatcgcattgatcgccaatgacctcacagtgcccgacttttccaacgccgaggtggagcggccgctggcggtcagcttgcccacccggcagtgcacctttgacaaggtgagtgcgctcaaacaggtgttggcgcgccaccccggcacctcgcaggtgcatctgcggctcatca</t>
         </is>
       </c>
     </row>
@@ -509,12 +509,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>G151C_Block-0</t>
+          <t>Y58N_Block-1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>cggtgccagcgagttctacaactccgcgaccaaggccgggatcaagccgatcatcggcgtggaggcatacatcgcgccgggctcgcggttcgacacccggcgcatcctgtggggtgaccccagccaaaaggccgacgacgtctccggcagcggctcctacacgcacctgacgatgatggccgagaacgccaccggtctgcgcaacctgttcaagctgtcctcgcatgcttccttcgagggccagctgagcaagtggtcgcgcatggacgccgagctcatcgccgaacacgccgagtgcatcatcatcaccaccggatgcccgtcgggggaggtgcagacccgcctgcggctcggccaggatcgggaggcgctcgaagccgcggcgaagtggcgggagatcgtcggaccggacaactacttccttgagctgatggaccacgggctgaccatcgaacgccgggtccgtgacggtctgctcgagatcggacgcgcgctcaacattccgcctcttgccaccaatgactgccactacgtgacccgcgacgccgcccacaaccatgaggctt</t>
+          <t>gatgcccgcggtggggatgaccgaccacggaaacatgttcggtgccagcgagttcaacaactccgcgaccaaggccgggatcaagccgatcatcggcgtggaggcatacatcgcgccgggctcgcggttcgacacccggcgcatcctgtggggtgaccccagccaaaaggccgacgacgtctccggcagcggctcctacacgcacctgacgatgatggccgagaacgccaccggtctgcgcaacctgttcaagctgtcctcgcatgcttccttcgagggccagctgagcaagtggtcgcgcatggacgccgagctcatcgccgaacacgccgagggcatcatcatcaccaccggatgcccgtcgggggaggtgcagacccgcctgcggctcggccaggatcgggaggcgctcgaagccgcggcgaagtggcgggagatcgtcggaccggacaactacttccttgagctgatggaccacgggctgaccatcgaacgccgggtccgtgacggtctgctcgagatcggacgcgcgctcaacattccgcctcttgccaccaatgactgccactacgtgacccgcgacgccgcccacaaccatgaggctttgttgtgtgtgcagaccggcaagaccctctcggatccgaatcgcttcaagttcgacggtgacggctactacctgaagtcggccgccgagatgcgccagatctgggacgacgaagtgccgggcgcgtgtgactccaccttgttgatcgccgaacgggtgcagtcctacgccgacgtgtggacaccgcgcgaccggatgcccgtgtttccggtgcccgatgggcatgaccaggcgtcctggctgcgtcacgaggtggacgccgggcttcgcc</t>
         </is>
       </c>
     </row>
@@ -526,12 +526,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>D574W_Block-2</t>
+          <t>C158S_Block-1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>cgcctacgcgctgggcatcaccgacatcgacccgattccacacggtctgctgttcgagcggttcctcaaccccgagcgcacctcgatgcccgacatcgatatcgacttcgacgaccggcgccgcggtgagatggtgcgctacgcagccgacaagtggggccacgaccgggtcgcgcaggtcatcaccttcggcaccatcaaaaccaaagcggcgctgaaggattcggcgcgaatccactacgggcagcccgggttcgccatcgccgaccggatcaccaaggcgttgccgccggcgatcatggccaaagacatcccgctgtctgggatcaccgatcccagccacgaacggtacaaggaggccgccgaggtccgcggcctgatcgaaaccgacccggacgtacgcaccatctaccagaccgcacgcgggttggaaggcctgatccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagcagcgagccgctgactgaggccatcccgttgtggaagcggccgcaggacggggccatcatcaccggctggtggtacccggcgtgcgaggccatcggtc</t>
+          <t>gatgcccgcggtggggatgaccgaccacggaaacatgttcggtgccagcgagttctacaactccgcgaccaaggccgggatcaagccgatcatcggcgtggaggcatacatcgcgccgggctcgcggttcgacacccggcgcatcctgtggggtgaccccagccaaaaggccgacgacgtctccggcagcggctcctacacgcacctgacgatgatggccgagaacgccaccggtctgcgcaacctgttcaagctgtcctcgcatgcttccttcgagggccagctgagcaagtggtcgcgcatggacgccgagctcatcgccgaacacgccgagggcatcatcatcaccaccggatcgccgtcgggggaggtgcagacccgcctgcggctcggccaggatcgggaggcgctcgaagccgcggcgaagtggcgggagatcgtcggaccggacaactacttccttgagctgatggaccacgggctgaccatcgaacgccgggtccgtgacggtctgctcgagatcggacgcgcgctcaacattccgcctcttgccaccaatgactgccactacgtgacccgcgacgccgcccacaaccatgaggctttgttgtgtgtgcagaccggcaagaccctctcggatccgaatcgcttcaagttcgacggtgacggctactacctgaagtcggccgccgagatgcgccagatctgggacgacgaagtgccgggcgcgtgtgactccaccttgttgatcgccgaacgggtgcagtcctacgccgacgtgtggacaccgcgcgaccggatgcccgtgtttccggtgcccgatgggcatgaccaggcgtcctggctgcgtcacgaggtggacgccgggcttcgcc</t>
         </is>
       </c>
     </row>
@@ -543,12 +543,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>A216K_Block-0</t>
+          <t>L217R_Block-1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>cggtgccagcgagttctacaactccgcgaccaaggccgggatcaagccgatcatcggcgtggaggcatacatcgcgccgggctcgcggttcgacacccggcgcatcctgtggggtgaccccagccaaaaggccgacgacgtctccggcagcggctcctacacgcacctgacgatgatggccgagaacgccaccggtctgcgcaacctgttcaagctgtcctcgcatgcttccttcgagggccagctgagcaagtggtcgcgcatggacgccgagctcatcgccgaacacgccgagggcatcatcatcaccaccggatgcccgtcgggggaggtgcagacccgcctgcggctcggccaggatcgggaggcgctcgaagccgcggcgaagtggcgggagatcgtcggaccggacaactacttccttgagctgatggaccacgggctgaccatcgaacgccgggtccgtgacggtctgctcgagatcggacgcaagctcaacattccgcctcttgccaccaatgactgccactacgtgacccgcgacgccgcccacaaccatgaggctt</t>
+          <t>gatgcccgcggtggggatgaccgaccacggaaacatgttcggtgccagcgagttctacaactccgcgaccaaggccgggatcaagccgatcatcggcgtggaggcatacatcgcgccgggctcgcggttcgacacccggcgcatcctgtggggtgaccccagccaaaaggccgacgacgtctccggcagcggctcctacacgcacctgacgatgatggccgagaacgccaccggtctgcgcaacctgttcaagctgtcctcgcatgcttccttcgagggccagctgagcaagtggtcgcgcatggacgccgagctcatcgccgaacacgccgagggcatcatcatcaccaccggatgcccgtcgggggaggtgcagacccgcctgcggctcggccaggatcgggaggcgctcgaagccgcggcgaagtggcgggagatcgtcggaccggacaactacttccttgagctgatggaccacgggctgaccatcgaacgccgggtccgtgacggtctgctcgagatcggacgcgcgcgcaacattccgcctcttgccaccaatgactgccactacgtgacccgcgacgccgcccacaaccatgaggctttgttgtgtgtgcagaccggcaagaccctctcggatccgaatcgcttcaagttcgacggtgacggctactacctgaagtcggccgccgagatgcgccagatctgggacgacgaagtgccgggcgcgtgtgactccaccttgttgatcgccgaacgggtgcagtcctacgccgacgtgtggacaccgcgcgaccggatgcccgtgtttccggtgcccgatgggcatgaccaggcgtcctggctgcgtcacgaggtggacgccgggcttcgcc</t>
         </is>
       </c>
     </row>
@@ -560,12 +560,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>G199D_Block-0</t>
+          <t>H919K_Block-3</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>cggtgccagcgagttctacaactccgcgaccaaggccgggatcaagccgatcatcggcgtggaggcatacatcgcgccgggctcgcggttcgacacccggcgcatcctgtggggtgaccccagccaaaaggccgacgacgtctccggcagcggctcctacacgcacctgacgatgatggccgagaacgccaccggtctgcgcaacctgttcaagctgtcctcgcatgcttccttcgagggccagctgagcaagtggtcgcgcatggacgccgagctcatcgccgaacacgccgagggcatcatcatcaccaccggatgcccgtcgggggaggtgcagacccgcctgcggctcggccaggatcgggaggcgctcgaagccgcggcgaagtggcgggagatcgtcggaccggacaactacttccttgagctgatggaccacgacctgaccatcgaacgccgggtccgtgacggtctgctcgagatcggacgcgcgctcaacattccgcctcttgccaccaatgactgccactacgtgacccgcgacgccgcccacaaccatgaggctt</t>
+          <t>cgacattctacgcaaggccatgggcaagaagaaacgcgaggtgctggagaaggagttcgagggcttctccgatggcatgcaggccaacgggttctctccggcggccatcaaggcgctgtgggacaccatcctgccgttcgctgactacgcgttcaacaagtcacatgccgccggctacggcatggtgtcctactggacggcctacctcaaggccaactatcccgccgagtacatggccggtctgttgacgtcggtcggcgacgataaagacaaggccgcggtttatctggccgactgccgcaagctcggcatcaccgtgctcccgcccgacgtcaacgaatctggcttgaacttcgcatcggtcggccaagacatccgctacgggctgggcgcggtgcgcaacgttggcgctaatgtcgtgggctcgttgctccaaacccgcaacgacaagggcaagttcaccgacttttcggactacctgaacaagatcgacatctcggcgtgcaacaagaaggtgaccgaatcgctgatcaaggcgggtgcgttcgactcgctggggaaggcccgcaagggtcttttcctggtgcacagcgatgcggtggactcggtgctgggcaccaagaaggccgaggcactggggcagttcgatctcttcggcagcaatgatgatgggaccggcaccgcagatcccgtgttcaccatcaaggtgcccgatgatgagtgggaggacaaacacaaactcgccctagagcgcgagatgctgggactgtacgtctcggggcatcccctcaacggtgtggcacacttgctggctgcccaggtcgacaccgcgatcccagcgatcctcgacggcgatgtccccaacgatgcccaagtgcgggtgggcggcatcctggcgtcggtgaaccggagggtcaacaaaaacggaatgccatgggcttcagcgcaattggaggatctcacgggcggcatcgaggtgatgttcttcccgcacacctactccagctatggtgccgacatcgtcgacgatgccgtcgtgctggtcaacgccaaggtggcggtccgtgacgaccgcatcgcattgatcgccaatgacctcacagtgcccgacttttccaacgccgaggtggagcggccgctggcggtcagcttgcccacccggcagtgcacctttgacaaggtgagtgcgctcaaacaggtgttggcgcgccaccccggcacctcgcaggtgcatctgcggctcatca</t>
         </is>
       </c>
     </row>
@@ -577,12 +577,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>D398Q_Block-2</t>
+          <t>R1135L_Block-3</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>cgcctacgcgctgggcatcacccagatcgacccgattccacacggtctgctgttcgagcggttcctcaaccccgagcgcacctcgatgcccgacatcgatatcgacttcgacgaccggcgccgcggtgagatggtgcgctacgcagccgacaagtggggccacgaccgggtcgcgcaggtcatcaccttcggcaccatcaaaaccaaagcggcgctgaaggattcggcgcgaatccactacgggcagcccgggttcgccatcgccgaccggatcaccaaggcgttgccgccggcgatcatggccaaagacatcccgctgtctgggatcaccgatcccagccacgaacggtacaaggaggccgccgaggtccgcggcctgatcgaaaccgacccggacgtacgcaccatctaccagaccgcacgcgggttggaaggcctgatccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagcagcgagccgctgactgaggccatcccgttgtggaagcggccgcaggacggggccatcatcaccggctgggattacccggcgtgcgaggccatcggtc</t>
+          <t>cgacattctacgcaaggccatgggcaagaagaaacgcgaggtgctggagaaggagttcgagggcttctccgatggcatgcaggccaacgggttctctccggcggccatcaaggcgctgtgggacaccatcctgccgttcgctgactacgcgttcaacaagtcacatgccgccggctacggcatggtgtcctactggacggcctacctcaaggccaactatcccgccgagtacatggccggtctgttgacgtcggtcggcgacgataaagacaaggccgcggtttatctggccgactgccgcaagctcggcatcaccgtgctcccgcccgacgtcaacgaatctggcttgaacttcgcatcggtcggccaagacatccgctacgggctgggcgcggtgcgcaacgttggcgctaatgtcgtgggctcgttgctccaaacccgcaacgacaagggcaagttcaccgacttttcggactacctgaacaagatcgacatctcggcgtgcaacaagaaggtgaccgaatcgctgatcaaggcgggtgcgttcgactcgctggggcatgcccgcaagggtcttttcctggtgcacagcgatgcggtggactcggtgctgggcaccaagaaggccgaggcactggggcagttcgatctcttcggcagcaatgatgatgggaccggcaccgcagatcccgtgttcaccatcaaggtgcccgatgatgagtgggaggacaaacacaaactcgccctagagcgcgagatgctgggactgtacgtctcggggcatcccctcaacggtgtggcacacttgctggctgcccaggtcgacaccgcgatcccagcgatcctcgacggcgatgtccccaacgatgcccaagtgcgggtgggcggcatcctggcgtcggtgaaccggagggtcaacaaaaacggaatgccatgggcttcagcgcaattggaggatctcacgggcggcatcgaggtgatgttcttcccgcacacctactccagctatggtgccgacatcgtcgacgatgccgtcgtgctggtcaacgccaaggtggcggtccgtgacgaccgcatcgcattgatcgccaatgacctcacagtgcccgacttttccaacgccgaggtggagcggccgctggcggtcagcttgcccacccggcagtgcacctttgacaaggtgagtgcgctcaaacaggtgttggcgctgcaccccggcacctcgcaggtgcatctgcggctcatca</t>
         </is>
       </c>
     </row>
@@ -594,12 +594,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>A789N_Block-4</t>
+          <t>T1139F_Block-3</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>gccgttcgctgactacgcgttcaacaagtcacatgccaacggctacggcatggtgtcctactggacggcctacctcaaggccaactatcccgccgagtacatggccggtctgttgacgtcggtcggcgacgataaagacaaggccgcggtttatctggccgactgccgcaagctcggcatcaccgtgctcccgcccgacgtcaacgaatctggcttgaacttcgcatcggtcggccaagacatccgctacgggctgggcgcggtgcgcaacgttggcgctaatgtcgtgggctcgttgctccaaacccgcaacgacaagggcaagttcaccgacttttcggactacctgaacaagatcgacatctcggcgtgcaacaagaaggtgaccgaatcgctgatcaaggcgggtgcgttcgactcgctggggcatgcccgcaagggtcttttcctggtgcacagcgatgcgg</t>
+          <t>cgacattctacgcaaggccatgggcaagaagaaacgcgaggtgctggagaaggagttcgagggcttctccgatggcatgcaggccaacgggttctctccggcggccatcaaggcgctgtgggacaccatcctgccgttcgctgactacgcgttcaacaagtcacatgccgccggctacggcatggtgtcctactggacggcctacctcaaggccaactatcccgccgagtacatggccggtctgttgacgtcggtcggcgacgataaagacaaggccgcggtttatctggccgactgccgcaagctcggcatcaccgtgctcccgcccgacgtcaacgaatctggcttgaacttcgcatcggtcggccaagacatccgctacgggctgggcgcggtgcgcaacgttggcgctaatgtcgtgggctcgttgctccaaacccgcaacgacaagggcaagttcaccgacttttcggactacctgaacaagatcgacatctcggcgtgcaacaagaaggtgaccgaatcgctgatcaaggcgggtgcgttcgactcgctggggcatgcccgcaagggtcttttcctggtgcacagcgatgcggtggactcggtgctgggcaccaagaaggccgaggcactggggcagttcgatctcttcggcagcaatgatgatgggaccggcaccgcagatcccgtgttcaccatcaaggtgcccgatgatgagtgggaggacaaacacaaactcgccctagagcgcgagatgctgggactgtacgtctcggggcatcccctcaacggtgtggcacacttgctggctgcccaggtcgacaccgcgatcccagcgatcctcgacggcgatgtccccaacgatgcccaagtgcgggtgggcggcatcctggcgtcggtgaaccggagggtcaacaaaaacggaatgccatgggcttcagcgcaattggaggatctcacgggcggcatcgaggtgatgttcttcccgcacacctactccagctatggtgccgacatcgtcgacgatgccgtcgtgctggtcaacgccaaggtggcggtccgtgacgaccgcatcgcattgatcgccaatgacctcacagtgcccgacttttccaacgccgaggtggagcggccgctggcggtcagcttgcccacccggcagtgcacctttgacaaggtgagtgcgctcaaacaggtgttggcgcgccaccccggcttctcgcaggtgcatctgcggctcatca</t>
         </is>
       </c>
     </row>
@@ -611,12 +611,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>I481L_Block-2</t>
+          <t>S1115P_Block-3</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>cgcctacgcgctgggcatcaccgacatcgacccgattccacacggtctgctgttcgagcggttcctcaaccccgagcgcacctcgatgcccgacatcgatatcgacttcgacgaccggcgccgcggtgagatggtgcgctacgcagccgacaagtggggccacgaccgggtcgcgcaggtcatcaccttcggcaccatcaaaaccaaagcggcgctgaaggattcggcgcgaatccactacgggcagcccgggttcgccatcgccgaccggctgaccaaggcgttgccgccggcgatcatggccaaagacatcccgctgtctgggatcaccgatcccagccacgaacggtacaaggaggccgccgaggtccgcggcctgatcgaaaccgacccggacgtacgcaccatctaccagaccgcacgcgggttggaaggcctgatccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagcagcgagccgctgactgaggccatcccgttgtggaagcggccgcaggacggggccatcatcaccggctgggattacccggcgtgcgaggccatcggtc</t>
+          <t>cgacattctacgcaaggccatgggcaagaagaaacgcgaggtgctggagaaggagttcgagggcttctccgatggcatgcaggccaacgggttctctccggcggccatcaaggcgctgtgggacaccatcctgccgttcgctgactacgcgttcaacaagtcacatgccgccggctacggcatggtgtcctactggacggcctacctcaaggccaactatcccgccgagtacatggccggtctgttgacgtcggtcggcgacgataaagacaaggccgcggtttatctggccgactgccgcaagctcggcatcaccgtgctcccgcccgacgtcaacgaatctggcttgaacttcgcatcggtcggccaagacatccgctacgggctgggcgcggtgcgcaacgttggcgctaatgtcgtgggctcgttgctccaaacccgcaacgacaagggcaagttcaccgacttttcggactacctgaacaagatcgacatctcggcgtgcaacaagaaggtgaccgaatcgctgatcaaggcgggtgcgttcgactcgctggggcatgcccgcaagggtcttttcctggtgcacagcgatgcggtggactcggtgctgggcaccaagaaggccgaggcactggggcagttcgatctcttcggcagcaatgatgatgggaccggcaccgcagatcccgtgttcaccatcaaggtgcccgatgatgagtgggaggacaaacacaaactcgccctagagcgcgagatgctgggactgtacgtctcggggcatcccctcaacggtgtggcacacttgctggctgcccaggtcgacaccgcgatcccagcgatcctcgacggcgatgtccccaacgatgcccaagtgcgggtgggcggcatcctggcgtcggtgaaccggagggtcaacaaaaacggaatgccatgggcttcagcgcaattggaggatctcacgggcggcatcgaggtgatgttcttcccgcacacctactccagctatggtgccgacatcgtcgacgatgccgtcgtgctggtcaacgccaaggtggcggtccgtgacgaccgcatcgcattgatcgccaatgacctcacagtgcccgacttttccaacgccgaggtggagcggccgctggcggtcccgttgcccacccggcagtgcacctttgacaaggtgagtgcgctcaaacaggtgttggcgcgccaccccggcacctcgcaggtgcatctgcggctcatca</t>
         </is>
       </c>
     </row>
@@ -628,12 +628,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>S991S_Block-6</t>
+          <t>I689I_Block-2</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>cgagatgctgggactgtacgtctcggggcatcccctcaacggtgtggcacacttgctggctgcccaggtcgacaccgcgatcccagcgatcctcgacggcgatgtccccaacgatgcccaagtgcgggtgggcggcatcctggcgtcggtgaaccggagggtcaacaaaaacggaatgccatgggcttcagcgcaattggaggatctcacgggcggcatcgaggtgatgttcttcccgcacacctactccagctatggtgccgacatcgtcgacgatgccgtcgtgctggtcaacgccaaggtggcggtccgtgacgaccgcatcgcattgatcgccaatgacctcacagtgcccgacttttccaacgccgaggtggagcggccgctggcggtcagcttgcccacccggcagtgcacctttgacaaggtgagtgcgctcaaacaggtgttggcgcgccaccccggcacct</t>
+          <t>gtactttctgatcgtcgccgacctgatcagctacgcgcggtcggcgggcataagggtgggtcccggccgcggctcggccgccggctcgctggtcgcctacgcgctgggcatcaccgacatcgacccgattccacacggtctgctgttcgagcggttcctcaaccccgagcgcacctcgatgcccgacatcgatatcgacttcgacgaccggcgccgcggtgagatggtgcgctacgcagccgacaagtggggccacgaccgggtcgcgcaggtcatcaccttcggcaccatcaaaaccaaagcggcgctgaaggattcggcgcgaatccactacgggcagcccgggttcgccatcgccgaccggatcaccaaggcgttgccgccggcgatcatggccaaagacatcccgctgtctgggatcaccgatcccagccacgaacggtacaaggaggccgccgaggtccgcggcctgatcgaaaccgacccggacgtacgcaccatctaccagaccgcacgcgggttggaaggcctgatccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagcagcgagccgctgactgaggccatcccgttgtggaagcggccgcaggacggggccatcatcaccggctgggattacccggcgtgcgaggccatcggtctgctgaaaatggacttcctgggcctgcggaacctgacgatcatcggcgacgcgatcgacaacgtcagggccaacaggggtatcgacctcgacctggaatccgtgccgctggacgacaaggccacctatgagctgctgggccgcggcgacaccctgggcgtgttccagctcgacggcgggcccatgcgcgacctgctgcgccgcatgcagccgaccgggttcgaagacgtcgtcgccgttatcgcgctgtaccggcccggcccgatgggcatgaacgcacacaacgactatgccgaccgcaagaacaaccggcaggccatcaaacctattcacccggaactcgaag</t>
         </is>
       </c>
     </row>
@@ -645,12 +645,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>N784H_Block-4</t>
+          <t>A931G_Block-3</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>gccgttcgctgactacgcgttccacaagtcacatgccgccggctacggcatggtgtcctactggacggcctacctcaaggccaactatcccgccgagtacatggccggtctgttgacgtcggtcggcgacgataaagacaaggccgcggtttatctggccgactgccgcaagctcggcatcaccgtgctcccgcccgacgtcaacgaatctggcttgaacttcgcatcggtcggccaagacatccgctacgggctgggcgcggtgcgcaacgttggcgctaatgtcgtgggctcgttgctccaaacccgcaacgacaagggcaagttcaccgacttttcggactacctgaacaagatcgacatctcggcgtgcaacaagaaggtgaccgaatcgctgatcaaggcgggtgcgttcgactcgctggggcatgcccgcaagggtcttttcctggtgcacagcgatgcgg</t>
+          <t>cgacattctacgcaaggccatgggcaagaagaaacgcgaggtgctggagaaggagttcgagggcttctccgatggcatgcaggccaacgggttctctccggcggccatcaaggcgctgtgggacaccatcctgccgttcgctgactacgcgttcaacaagtcacatgccgccggctacggcatggtgtcctactggacggcctacctcaaggccaactatcccgccgagtacatggccggtctgttgacgtcggtcggcgacgataaagacaaggccgcggtttatctggccgactgccgcaagctcggcatcaccgtgctcccgcccgacgtcaacgaatctggcttgaacttcgcatcggtcggccaagacatccgctacgggctgggcgcggtgcgcaacgttggcgctaatgtcgtgggctcgttgctccaaacccgcaacgacaagggcaagttcaccgacttttcggactacctgaacaagatcgacatctcggcgtgcaacaagaaggtgaccgaatcgctgatcaaggcgggtgcgttcgactcgctggggcatgcccgcaagggtcttttcctggtgcacagcgatggcgtggactcggtgctgggcaccaagaaggccgaggcactggggcagttcgatctcttcggcagcaatgatgatgggaccggcaccgcagatcccgtgttcaccatcaaggtgcccgatgatgagtgggaggacaaacacaaactcgccctagagcgcgagatgctgggactgtacgtctcggggcatcccctcaacggtgtggcacacttgctggctgcccaggtcgacaccgcgatcccagcgatcctcgacggcgatgtccccaacgatgcccaagtgcgggtgggcggcatcctggcgtcggtgaaccggagggtcaacaaaaacggaatgccatgggcttcagcgcaattggaggatctcacgggcggcatcgaggtgatgttcttcccgcacacctactccagctatggtgccgacatcgtcgacgatgccgtcgtgctggtcaacgccaaggtggcggtccgtgacgaccgcatcgcattgatcgccaatgacctcacagtgcccgacttttccaacgccgaggtggagcggccgctggcggtcagcttgcccacccggcagtgcacctttgacaaggtgagtgcgctcaaacaggtgttggcgcgccaccccggcacctcgcaggtgcatctgcggctcatca</t>
         </is>
       </c>
     </row>
@@ -662,12 +662,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>R1035P_Block-6</t>
+          <t>D47Y_Block-1</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>cgagatgctgggactgtacgtctcggggcatcccctcaacggtgtggcacacttgctggctgcccaggtcgacaccgcgatcccagcgatcctcgacggcgatgtccccaacgatgcccaagtgcgggtgggcggcatcctggcgtcggtgaacccgagggtcaacaaaaacggaatgccatgggcttcagcgcaattggaggatctcacgggcggcatcgaggtgatgttcttcccgcacacctactccagctatggtgccgacatcgtcgacgatgccgtcgtgctggtcaacgccaaggtggcggtccgtgacgaccgcatcgcattgatcgccaatgacctcacagtgcccgacttttccaacgccgaggtggagcggccgctggcggtcagcttgcccacccggcagtgcacctttgacaaggtgagtgcgctcaaacaggtgttggcgcgccaccccggcacct</t>
+          <t>gatgcccgcggtggggatgacctaccacggaaacatgttcggtgccagcgagttctacaactccgcgaccaaggccgggatcaagccgatcatcggcgtggaggcatacatcgcgccgggctcgcggttcgacacccggcgcatcctgtggggtgaccccagccaaaaggccgacgacgtctccggcagcggctcctacacgcacctgacgatgatggccgagaacgccaccggtctgcgcaacctgttcaagctgtcctcgcatgcttccttcgagggccagctgagcaagtggtcgcgcatggacgccgagctcatcgccgaacacgccgagggcatcatcatcaccaccggatgcccgtcgggggaggtgcagacccgcctgcggctcggccaggatcgggaggcgctcgaagccgcggcgaagtggcgggagatcgtcggaccggacaactacttccttgagctgatggaccacgggctgaccatcgaacgccgggtccgtgacggtctgctcgagatcggacgcgcgctcaacattccgcctcttgccaccaatgactgccactacgtgacccgcgacgccgcccacaaccatgaggctttgttgtgtgtgcagaccggcaagaccctctcggatccgaatcgcttcaagttcgacggtgacggctactacctgaagtcggccgccgagatgcgccagatctgggacgacgaagtgccgggcgcgtgtgactccaccttgttgatcgccgaacgggtgcagtcctacgccgacgtgtggacaccgcgcgaccggatgcccgtgtttccggtgcccgatgggcatgaccaggcgtcctggctgcgtcacgaggtggacgccgggcttcgcc</t>
         </is>
       </c>
     </row>
@@ -679,12 +679,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>A180E_Block-0</t>
+          <t>R322Q_Block-1</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>cggtgccagcgagttctacaactccgcgaccaaggccgggatcaagccgatcatcggcgtggaggcatacatcgcgccgggctcgcggttcgacacccggcgcatcctgtggggtgaccccagccaaaaggccgacgacgtctccggcagcggctcctacacgcacctgacgatgatggccgagaacgccaccggtctgcgcaacctgttcaagctgtcctcgcatgcttccttcgagggccagctgagcaagtggtcgcgcatggacgccgagctcatcgccgaacacgccgagggcatcatcatcaccaccggatgcccgtcgggggaggtgcagacccgcctgcggctcggccaggatcgggaggcgctcgaagccgcggagaagtggcgggagatcgtcggaccggacaactacttccttgagctgatggaccacgggctgaccatcgaacgccgggtccgtgacggtctgctcgagatcggacgcgcgctcaacattccgcctcttgccaccaatgactgccactacgtgacccgcgacgccgcccacaaccatgaggctt</t>
+          <t>gatgcccgcggtggggatgaccgaccacggaaacatgttcggtgccagcgagttctacaactccgcgaccaaggccgggatcaagccgatcatcggcgtggaggcatacatcgcgccgggctcgcggttcgacacccggcgcatcctgtggggtgaccccagccaaaaggccgacgacgtctccggcagcggctcctacacgcacctgacgatgatggccgagaacgccaccggtctgcgcaacctgttcaagctgtcctcgcatgcttccttcgagggccagctgagcaagtggtcgcgcatggacgccgagctcatcgccgaacacgccgagggcatcatcatcaccaccggatgcccgtcgggggaggtgcagacccgcctgcggctcggccaggatcgggaggcgctcgaagccgcggcgaagtggcgggagatcgtcggaccggacaactacttccttgagctgatggaccacgggctgaccatcgaacgccgggtccgtgacggtctgctcgagatcggacgcgcgctcaacattccgcctcttgccaccaatgactgccactacgtgacccgcgacgccgcccacaaccatgaggctttgttgtgtgtgcagaccggcaagaccctctcggatccgaatcgcttcaagttcgacggtgacggctactacctgaagtcggccgccgagatgcgccagatctgggacgacgaagtgccgggcgcgtgtgactccaccttgttgatcgccgaacgggtgcagtcctacgccgacgtgtggacaccgcgcgaccggatgcccgtgtttccggtgcccgatgggcatgaccaggcgtcctggctgcagcacgaggtggacgccgggcttcgcc</t>
         </is>
       </c>
     </row>
@@ -696,12 +696,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>A484V_Block-2</t>
+          <t>G740C_Block-3</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>cgcctacgcgctgggcatcaccgacatcgacccgattccacacggtctgctgttcgagcggttcctcaaccccgagcgcacctcgatgcccgacatcgatatcgacttcgacgaccggcgccgcggtgagatggtgcgctacgcagccgacaagtggggccacgaccgggtcgcgcaggtcatcaccttcggcaccatcaaaaccaaagcggcgctgaaggattcggcgcgaatccactacgggcagcccgggttcgccatcgccgaccggatcaccaaggtgttgccgccggcgatcatggccaaagacatcccgctgtctgggatcaccgatcccagccacgaacggtacaaggaggccgccgaggtccgcggcctgatcgaaaccgacccggacgtacgcaccatctaccagaccgcacgcgggttggaaggcctgatccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagcagcgagccgctgactgaggccatcccgttgtggaagcggccgcaggacggggccatcatcaccggctgggattacccggcgtgcgaggccatcggtc</t>
+          <t>cgacattctacgcaaggccatgtgcaagaagaaacgcgaggtgctggagaaggagttcgagggcttctccgatggcatgcaggccaacgggttctctccggcggccatcaaggcgctgtgggacaccatcctgccgttcgctgactacgcgttcaacaagtcacatgccgccggctacggcatggtgtcctactggacggcctacctcaaggccaactatcccgccgagtacatggccggtctgttgacgtcggtcggcgacgataaagacaaggccgcggtttatctggccgactgccgcaagctcggcatcaccgtgctcccgcccgacgtcaacgaatctggcttgaacttcgcatcggtcggccaagacatccgctacgggctgggcgcggtgcgcaacgttggcgctaatgtcgtgggctcgttgctccaaacccgcaacgacaagggcaagttcaccgacttttcggactacctgaacaagatcgacatctcggcgtgcaacaagaaggtgaccgaatcgctgatcaaggcgggtgcgttcgactcgctggggcatgcccgcaagggtcttttcctggtgcacagcgatgcggtggactcggtgctgggcaccaagaaggccgaggcactggggcagttcgatctcttcggcagcaatgatgatgggaccggcaccgcagatcccgtgttcaccatcaaggtgcccgatgatgagtgggaggacaaacacaaactcgccctagagcgcgagatgctgggactgtacgtctcggggcatcccctcaacggtgtggcacacttgctggctgcccaggtcgacaccgcgatcccagcgatcctcgacggcgatgtccccaacgatgcccaagtgcgggtgggcggcatcctggcgtcggtgaaccggagggtcaacaaaaacggaatgccatgggcttcagcgcaattggaggatctcacgggcggcatcgaggtgatgttcttcccgcacacctactccagctatggtgccgacatcgtcgacgatgccgtcgtgctggtcaacgccaaggtggcggtccgtgacgaccgcatcgcattgatcgccaatgacctcacagtgcccgacttttccaacgccgaggtggagcggccgctggcggtcagcttgcccacccggcagtgcacctttgacaaggtgagtgcgctcaaacaggtgttggcgcgccaccccggcacctcgcaggtgcatctgcggctcatca</t>
         </is>
       </c>
     </row>
@@ -713,12 +713,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>G498G_Block-2</t>
+          <t>V817H_Block-3</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>cgcctacgcgctgggcatcaccgacatcgacccgattccacacggtctgctgttcgagcggttcctcaaccccgagcgcacctcgatgcccgacatcgatatcgacttcgacgaccggcgccgcggtgagatggtgcgctacgcagccgacaagtggggccacgaccgggtcgcgcaggtcatcaccttcggcaccatcaaaaccaaagcggcgctgaaggattcggcgcgaatccactacgggcagcccgggttcgccatcgccgaccggatcaccaaggcgttgccgccggcgatcatggccaaagacatcccgctgtctggcatcaccgatcccagccacgaacggtacaaggaggccgccgaggtccgcggcctgatcgaaaccgacccggacgtacgcaccatctaccagaccgcacgcgggttggaaggcctgatccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagcagcgagccgctgactgaggccatcccgttgtggaagcggccgcaggacggggccatcatcaccggctgggattacccggcgtgcgaggccatcggtc</t>
+          <t>cgacattctacgcaaggccatgggcaagaagaaacgcgaggtgctggagaaggagttcgagggcttctccgatggcatgcaggccaacgggttctctccggcggccatcaaggcgctgtgggacaccatcctgccgttcgctgactacgcgttcaacaagtcacatgccgccggctacggcatggtgtcctactggacggcctacctcaaggccaactatcccgccgagtacatggccggtctgttgacgtcgcacggcgacgataaagacaaggccgcggtttatctggccgactgccgcaagctcggcatcaccgtgctcccgcccgacgtcaacgaatctggcttgaacttcgcatcggtcggccaagacatccgctacgggctgggcgcggtgcgcaacgttggcgctaatgtcgtgggctcgttgctccaaacccgcaacgacaagggcaagttcaccgacttttcggactacctgaacaagatcgacatctcggcgtgcaacaagaaggtgaccgaatcgctgatcaaggcgggtgcgttcgactcgctggggcatgcccgcaagggtcttttcctggtgcacagcgatgcggtggactcggtgctgggcaccaagaaggccgaggcactggggcagttcgatctcttcggcagcaatgatgatgggaccggcaccgcagatcccgtgttcaccatcaaggtgcccgatgatgagtgggaggacaaacacaaactcgccctagagcgcgagatgctgggactgtacgtctcggggcatcccctcaacggtgtggcacacttgctggctgcccaggtcgacaccgcgatcccagcgatcctcgacggcgatgtccccaacgatgcccaagtgcgggtgggcggcatcctggcgtcggtgaaccggagggtcaacaaaaacggaatgccatgggcttcagcgcaattggaggatctcacgggcggcatcgaggtgatgttcttcccgcacacctactccagctatggtgccgacatcgtcgacgatgccgtcgtgctggtcaacgccaaggtggcggtccgtgacgaccgcatcgcattgatcgccaatgacctcacagtgcccgacttttccaacgccgaggtggagcggccgctggcggtcagcttgcccacccggcagtgcacctttgacaaggtgagtgcgctcaaacaggtgttggcgcgccaccccggcacctcgcaggtgcatctgcggctcatca</t>
         </is>
       </c>
     </row>
@@ -730,12 +730,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>R204F_Block-0</t>
+          <t>E150V_Block-1</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>cggtgccagcgagttctacaactccgcgaccaaggccgggatcaagccgatcatcggcgtggaggcatacatcgcgccgggctcgcggttcgacacccggcgcatcctgtggggtgaccccagccaaaaggccgacgacgtctccggcagcggctcctacacgcacctgacgatgatggccgagaacgccaccggtctgcgcaacctgttcaagctgtcctcgcatgcttccttcgagggccagctgagcaagtggtcgcgcatggacgccgagctcatcgccgaacacgccgagggcatcatcatcaccaccggatgcccgtcgggggaggtgcagacccgcctgcggctcggccaggatcgggaggcgctcgaagccgcggcgaagtggcgggagatcgtcggaccggacaactacttccttgagctgatggaccacgggctgaccatcgaattccgggtccgtgacggtctgctcgagatcggacgcgcgctcaacattccgcctcttgccaccaatgactgccactacgtgacccgcgacgccgcccacaaccatgaggctt</t>
+          <t>gatgcccgcggtggggatgaccgaccacggaaacatgttcggtgccagcgagttctacaactccgcgaccaaggccgggatcaagccgatcatcggcgtggaggcatacatcgcgccgggctcgcggttcgacacccggcgcatcctgtggggtgaccccagccaaaaggccgacgacgtctccggcagcggctcctacacgcacctgacgatgatggccgagaacgccaccggtctgcgcaacctgttcaagctgtcctcgcatgcttccttcgagggccagctgagcaagtggtcgcgcatggacgccgagctcatcgccgaacacgccgtgggcatcatcatcaccaccggatgcccgtcgggggaggtgcagacccgcctgcggctcggccaggatcgggaggcgctcgaagccgcggcgaagtggcgggagatcgtcggaccggacaactacttccttgagctgatggaccacgggctgaccatcgaacgccgggtccgtgacggtctgctcgagatcggacgcgcgctcaacattccgcctcttgccaccaatgactgccactacgtgacccgcgacgccgcccacaaccatgaggctttgttgtgtgtgcagaccggcaagaccctctcggatccgaatcgcttcaagttcgacggtgacggctactacctgaagtcggccgccgagatgcgccagatctgggacgacgaagtgccgggcgcgtgtgactccaccttgttgatcgccgaacgggtgcagtcctacgccgacgtgtggacaccgcgcgaccggatgcccgtgtttccggtgcccgatgggcatgaccaggcgtcctggctgcgtcacgaggtggacgccgggcttcgcc</t>
         </is>
       </c>
     </row>
@@ -747,12 +747,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>R232M_Block-0</t>
+          <t>L367M_Block-2</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>cggtgccagcgagttctacaactccgcgaccaaggccgggatcaagccgatcatcggcgtggaggcatacatcgcgccgggctcgcggttcgacacccggcgcatcctgtggggtgaccccagccaaaaggccgacgacgtctccggcagcggctcctacacgcacctgacgatgatggccgagaacgccaccggtctgcgcaacctgttcaagctgtcctcgcatgcttccttcgagggccagctgagcaagtggtcgcgcatggacgccgagctcatcgccgaacacgccgagggcatcatcatcaccaccggatgcccgtcgggggaggtgcagacccgcctgcggctcggccaggatcgggaggcgctcgaagccgcggcgaagtggcgggagatcgtcggaccggacaactacttccttgagctgatggaccacgggctgaccatcgaacgccgggtccgtgacggtctgctcgagatcggacgcgcgctcaacattccgcctcttgccaccaatgactgccactacgtgaccatggacgccgcccacaaccatgaggctt</t>
+          <t>gtactttctgatcgtcgccgacatgatcagctacgcgcggtcggcgggcataagggtgggtcccggccgcggctcggccgccggctcgctggtcgcctacgcgctgggcatcaccgacatcgacccgattccacacggtctgctgttcgagcggttcctcaaccccgagcgcacctcgatgcccgacatcgatatcgacttcgacgaccggcgccgcggtgagatggtgcgctacgcagccgacaagtggggccacgaccgggtcgcgcaggtcatcaccttcggcaccatcaaaaccaaagcggcgctgaaggattcggcgcgaatccactacgggcagcccgggttcgccatcgccgaccggatcaccaaggcgttgccgccggcgatcatggccaaagacatcccgctgtctgggatcaccgatcccagccacgaacggtacaaggaggccgccgaggtccgcggcctgatcgaaaccgacccggacgtacgcaccatctaccagaccgcacgcgggttggaaggcctgatccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagcagcgagccgctgactgaggccatcccgttgtggaagcggccgcaggacggggccatcatcaccggctgggattacccggcgtgcgaggccatcggtctgctgaaaatggacttcctgggcctgcggaacctgacgatcatcggcgacgcgatcgacaacgtcagggccaacaggggtatcgacctcgacctggaatccgtgccgctggacgacaaggccacctatgagctgctgggccgcggcgacaccctgggcgtgttccagctcgacggcgggcccatgcgcgacctgctgcgccgcatgcagccgaccgggttcgaagacgtcgtcgccgttatcgcgctgtaccggcccggcccgatgggcatgaacgcacacaacgactatgccgaccgcaagaacaaccggcaggccatcaaacctattcacccggaactcgaag</t>
         </is>
       </c>
     </row>
@@ -764,12 +764,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>G923A_Block-4</t>
+          <t>H236D_Block-1</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>gccgttcgctgactacgcgttcaacaagtcacatgccgccggctacggcatggtgtcctactggacggcctacctcaaggccaactatcccgccgagtacatggccggtctgttgacgtcggtcggcgacgataaagacaaggccgcggtttatctggccgactgccgcaagctcggcatcaccgtgctcccgcccgacgtcaacgaatctggcttgaacttcgcatcggtcggccaagacatccgctacgggctgggcgcggtgcgcaacgttggcgctaatgtcgtgggctcgttgctccaaacccgcaacgacaagggcaagttcaccgacttttcggactacctgaacaagatcgacatctcggcgtgcaacaagaaggtgaccgaatcgctgatcaaggcgggtgcgttcgactcgctggggcatgcccgcaaggcccttttcctggtgcacagcgatgcgg</t>
+          <t>gatgcccgcggtggggatgaccgaccacggaaacatgttcggtgccagcgagttctacaactccgcgaccaaggccgggatcaagccgatcatcggcgtggaggcatacatcgcgccgggctcgcggttcgacacccggcgcatcctgtggggtgaccccagccaaaaggccgacgacgtctccggcagcggctcctacacgcacctgacgatgatggccgagaacgccaccggtctgcgcaacctgttcaagctgtcctcgcatgcttccttcgagggccagctgagcaagtggtcgcgcatggacgccgagctcatcgccgaacacgccgagggcatcatcatcaccaccggatgcccgtcgggggaggtgcagacccgcctgcggctcggccaggatcgggaggcgctcgaagccgcggcgaagtggcgggagatcgtcggaccggacaactacttccttgagctgatggaccacgggctgaccatcgaacgccgggtccgtgacggtctgctcgagatcggacgcgcgctcaacattccgcctcttgccaccaatgactgccactacgtgacccgcgacgccgccgacaaccatgaggctttgttgtgtgtgcagaccggcaagaccctctcggatccgaatcgcttcaagttcgacggtgacggctactacctgaagtcggccgccgagatgcgccagatctgggacgacgaagtgccgggcgcgtgtgactccaccttgttgatcgccgaacgggtgcagtcctacgccgacgtgtggacaccgcgcgaccggatgcccgtgtttccggtgcccgatgggcatgaccaggcgtcctggctgcgtcacgaggtggacgccgggcttcgcc</t>
         </is>
       </c>
     </row>
@@ -781,12 +781,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Q1131Y_Block-6</t>
+          <t>N218A_Block-1</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>cgagatgctgggactgtacgtctcggggcatcccctcaacggtgtggcacacttgctggctgcccaggtcgacaccgcgatcccagcgatcctcgacggcgatgtccccaacgatgcccaagtgcgggtgggcggcatcctggcgtcggtgaaccggagggtcaacaaaaacggaatgccatgggcttcagcgcaattggaggatctcacgggcggcatcgaggtgatgttcttcccgcacacctactccagctatggtgccgacatcgtcgacgatgccgtcgtgctggtcaacgccaaggtggcggtccgtgacgaccgcatcgcattgatcgccaatgacctcacagtgcccgacttttccaacgccgaggtggagcggccgctggcggtcagcttgcccacccggcagtgcacctttgacaaggtgagtgcgctcaaatacgtgttggcgcgccaccccggcacct</t>
+          <t>gatgcccgcggtggggatgaccgaccacggaaacatgttcggtgccagcgagttctacaactccgcgaccaaggccgggatcaagccgatcatcggcgtggaggcatacatcgcgccgggctcgcggttcgacacccggcgcatcctgtggggtgaccccagccaaaaggccgacgacgtctccggcagcggctcctacacgcacctgacgatgatggccgagaacgccaccggtctgcgcaacctgttcaagctgtcctcgcatgcttccttcgagggccagctgagcaagtggtcgcgcatggacgccgagctcatcgccgaacacgccgagggcatcatcatcaccaccggatgcccgtcgggggaggtgcagacccgcctgcggctcggccaggatcgggaggcgctcgaagccgcggcgaagtggcgggagatcgtcggaccggacaactacttccttgagctgatggaccacgggctgaccatcgaacgccgggtccgtgacggtctgctcgagatcggacgcgcgctcgccattccgcctcttgccaccaatgactgccactacgtgacccgcgacgccgcccacaaccatgaggctttgttgtgtgtgcagaccggcaagaccctctcggatccgaatcgcttcaagttcgacggtgacggctactacctgaagtcggccgccgagatgcgccagatctgggacgacgaagtgccgggcgcgtgtgactccaccttgttgatcgccgaacgggtgcagtcctacgccgacgtgtggacaccgcgcgaccggatgcccgtgtttccggtgcccgatgggcatgaccaggcgtcctggctgcgtcacgaggtggacgccgggcttcgcc</t>
         </is>
       </c>
     </row>
@@ -798,12 +798,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Y105S-M111F_Block-0</t>
+          <t>A530K-L560K-A557H-P559N_Block-2</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>cggtgccagcgagttctacaactccgcgaccaaggccgggatcaagccgatcatcggcgtggaggcatacatcgcgccgggctcgcggttcgacacccggcgcatcctgtggggtgaccccagccaaaaggccgacgacgtctccggcagcggctcctcgacgcacctgacgatgttcgccgagaacgccaccggtctgcgcaacctgttcaagctgtcctcgcatgcttccttcgagggccagctgagcaagtggtcgcgcatggacgccgagctcatcgccgaacacgccgagggcatcatcatcaccaccggatgcccgtcgggggaggtgcagacccgcctgcggctcggccaggatcgggaggcgctcgaagccgcggcgaagtggcgggagatcgtcggaccggacaactacttccttgagctgatggaccacgggctgaccatcgaacgccgggtccgtgacggtctgctcgagatcggacgcgcgctcaacattccgcctcttgccaccaatgactgccactacgtgacccgcgacgccgcccacaaccatgaggctt</t>
+          <t>gtactttctgatcgtcgccgacctgatcagctacgcgcggtcggcgggcataagggtgggtcccggccgcggctcggccgccggctcgctggtcgcctacgcgctgggcatcaccgacatcgacccgattccacacggtctgctgttcgagcggttcctcaaccccgagcgcacctcgatgcccgacatcgatatcgacttcgacgaccggcgccgcggtgagatggtgcgctacgcagccgacaagtggggccacgaccgggtcgcgcaggtcatcaccttcggcaccatcaaaaccaaagcggcgctgaaggattcggcgcgaatccactacgggcagcccgggttcgccatcgccgaccggatcaccaaggcgttgccgccggcgatcatggccaaagacatcccgctgtctgggatcaccgatcccagccacgaacggtacaaggaggccgccgaggtccgcggcctgatcgaaaccgacccggacgtacgcaccatctaccagaccaagcgcgggttggaaggcctgatccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagcagcgagccgctgactgagcacatcaacaagtggaagcggccgcaggacggggccatcatcaccggctgggattacccggcgtgcgaggccatcggtctgctgaaaatggacttcctgggcctgcggaacctgacgatcatcggcgacgcgatcgacaacgtcagggccaacaggggtatcgacctcgacctggaatccgtgccgctggacgacaaggccacctatgagctgctgggccgcggcgacaccctgggcgtgttccagctcgacggcgggcccatgcgcgacctgctgcgccgcatgcagccgaccgggttcgaagacgtcgtcgccgttatcgcgctgtaccggcccggcccgatgggcatgaacgcacacaacgactatgccgaccgcaagaacaaccggcaggccatcaaacctattcacccggaactcgaag</t>
         </is>
       </c>
     </row>
@@ -815,12 +815,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>S100F-M110Q_Block-0</t>
+          <t>T957F-L986K-E984M-M985E_Block-3</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>cggtgccagcgagttctacaactccgcgaccaaggccgggatcaagccgatcatcggcgtggaggcatacatcgcgccgggctcgcggttcgacacccggcgcatcctgtggggtgaccccagccaaaaggccgacgacgtcttcggcagcggctcctacacgcacctgacgcagatggccgagaacgccaccggtctgcgcaacctgttcaagctgtcctcgcatgcttccttcgagggccagctgagcaagtggtcgcgcatggacgccgagctcatcgccgaacacgccgagggcatcatcatcaccaccggatgcccgtcgggggaggtgcagacccgcctgcggctcggccaggatcgggaggcgctcgaagccgcggcgaagtggcgggagatcgtcggaccggacaactacttccttgagctgatggaccacgggctgaccatcgaacgccgggtccgtgacggtctgctcgagatcggacgcgcgctcaacattccgcctcttgccaccaatgactgccactacgtgacccgcgacgccgcccacaaccatgaggctt</t>
+          <t>cgacattctacgcaaggccatgggcaagaagaaacgcgaggtgctggagaaggagttcgagggcttctccgatggcatgcaggccaacgggttctctccggcggccatcaaggcgctgtgggacaccatcctgccgttcgctgactacgcgttcaacaagtcacatgccgccggctacggcatggtgtcctactggacggcctacctcaaggccaactatcccgccgagtacatggccggtctgttgacgtcggtcggcgacgataaagacaaggccgcggtttatctggccgactgccgcaagctcggcatcaccgtgctcccgcccgacgtcaacgaatctggcttgaacttcgcatcggtcggccaagacatccgctacgggctgggcgcggtgcgcaacgttggcgctaatgtcgtgggctcgttgctccaaacccgcaacgacaagggcaagttcaccgacttttcggactacctgaacaagatcgacatctcggcgtgcaacaagaaggtgaccgaatcgctgatcaaggcgggtgcgttcgactcgctggggcatgcccgcaagggtcttttcctggtgcacagcgatgcggtggactcggtgctgggcaccaagaaggccgaggcactggggcagttcgatctcttcggcagcaatgatgatgggttcggcaccgcagatcccgtgttcaccatcaaggtgcccgatgatgagtgggaggacaaacacaaactcgccctagagcgcatggagaagggactgtacgtctcggggcatcccctcaacggtgtggcacacttgctggctgcccaggtcgacaccgcgatcccagcgatcctcgacggcgatgtccccaacgatgcccaagtgcgggtgggcggcatcctggcgtcggtgaaccggagggtcaacaaaaacggaatgccatgggcttcagcgcaattggaggatctcacgggcggcatcgaggtgatgttcttcccgcacacctactccagctatggtgccgacatcgtcgacgatgccgtcgtgctggtcaacgccaaggtggcggtccgtgacgaccgcatcgcattgatcgccaatgacctcacagtgcccgacttttccaacgccgaggtggagcggccgctggcggtcagcttgcccacccggcagtgcacctttgacaaggtgagtgcgctcaaacaggtgttggcgcgccaccccggcacctcgcaggtgcatctgcggctcatca</t>
         </is>
       </c>
     </row>
@@ -832,12 +832,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>S60-YWVGSC_Block-0</t>
+          <t>V1018-YDCG_Block-3</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>cggtgccagcgagttctacaactcctactgggtgggctcgtgcgcgaccaaggccgggatcaagccgatcatcggcgtggaggcatacatcgcgccgggctcgcggttcgacacccggcgcatcctgtggggtgaccccagccaaaaggccgacgacgtctccggcagcggctcctacacgcacctgacgatgatggccgagaacgccaccggtctgcgcaacctgttcaagctgtcctcgcatgcttccttcgagggccagctgagcaagtggtcgcgcatggacgccgagctcatcgccgaacacgccgagggcatcatcatcaccaccggatgcccgtcgggggaggtgcagacccgcctgcggctcggccaggatcgggaggcgctcgaagccgcggcgaagtggcgggagatcgtcggaccggacaactacttccttgagctgatggaccacgggctgaccatcgaacgccgggtccgtgacggtctgctcgagatcggacgcgcgctcaacattccgcctcttgccaccaatgactgccactacgtgacccgcgacgccgcccacaaccatgaggctt</t>
+          <t>cgacattctacgcaaggccatgggcaagaagaaacgcgaggtgctggagaaggagttcgagggcttctccgatggcatgcaggccaacgggttctctccggcggccatcaaggcgctgtgggacaccatcctgccgttcgctgactacgcgttcaacaagtcacatgccgccggctacggcatggtgtcctactggacggcctacctcaaggccaactatcccgccgagtacatggccggtctgttgacgtcggtcggcgacgataaagacaaggccgcggtttatctggccgactgccgcaagctcggcatcaccgtgctcccgcccgacgtcaacgaatctggcttgaacttcgcatcggtcggccaagacatccgctacgggctgggcgcggtgcgcaacgttggcgctaatgtcgtgggctcgttgctccaaacccgcaacgacaagggcaagttcaccgacttttcggactacctgaacaagatcgacatctcggcgtgcaacaagaaggtgaccgaatcgctgatcaaggcgggtgcgttcgactcgctggggcatgcccgcaagggtcttttcctggtgcacagcgatgcggtggactcggtgctgggcaccaagaaggccgaggcactggggcagttcgatctcttcggcagcaatgatgatgggaccggcaccgcagatcccgtgttcaccatcaaggtgcccgatgatgagtgggaggacaaacacaaactcgccctagagcgcgagatgctgggactgtacgtctcggggcatcccctcaacggtgtggcacacttgctggctgcccaggtcgacaccgcgatcccagcgatcctcgacggcgatgtctacgactgcggccccaacgatgcccaagtgcgggtgggcggcatcctggcgtcggtgaaccggagggtcaacaaaaacggaatgccatgggcttcagcgcaattggaggatctcacgggcggcatcgaggtgatgttcttcccgcacacctactccagctatggtgccgacatcgtcgacgatgccgtcgtgctggtcaacgccaaggtggcggtccgtgacgaccgcatcgcattgatcgccaatgacctcacagtgcccgacttttccaacgccgaggtggagcggccgctggcggtcagcttgcccacccggcagtgcacctttgacaaggtgagtgcgctcaaacaggtgttggcgcgccaccccggcacctcgcaggtgcatctgcggctcatca</t>
         </is>
       </c>
     </row>
@@ -849,12 +849,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>D428-CSGR_Block-2</t>
+          <t>V843-MDKHVC_Block-3</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>cgcctacgcgctgggcatcaccgacatcgacccgattccacacggtctgctgttcgagcggttcctcaaccccgagcgcacctcgatgcccgacatcgatatcgacttcgacgactgctcgggccgccggcgccgcggtgagatggtgcgctacgcagccgacaagtggggccacgaccgggtcgcgcaggtcatcaccttcggcaccatcaaaaccaaagcggcgctgaaggattcggcgcgaatccactacgggcagcccgggttcgccatcgccgaccggatcaccaaggcgttgccgccggcgatcatggccaaagacatcccgctgtctgggatcaccgatcccagccacgaacggtacaaggaggccgccgaggtccgcggcctgatcgaaaccgacccggacgtacgcaccatctaccagaccgcacgcgggttggaaggcctgatccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagcagcgagccgctgactgaggccatcccgttgtggaagcggccgcaggacggggccatcatcaccggctgggattacccggcgtgcgaggccatcggtc</t>
+          <t>cgacattctacgcaaggccatgggcaagaagaaacgcgaggtgctggagaaggagttcgagggcttctccgatggcatgcaggccaacgggttctctccggcggccatcaaggcgctgtgggacaccatcctgccgttcgctgactacgcgttcaacaagtcacatgccgccggctacggcatggtgtcctactggacggcctacctcaaggccaactatcccgccgagtacatggccggtctgttgacgtcggtcggcgacgataaagacaaggccgcggtttatctggccgactgccgcaagctcggcatcaccgtgctcccgcccgacgtcatggacaagcacgtgtgcaacgaatctggcttgaacttcgcatcggtcggccaagacatccgctacgggctgggcgcggtgcgcaacgttggcgctaatgtcgtgggctcgttgctccaaacccgcaacgacaagggcaagttcaccgacttttcggactacctgaacaagatcgacatctcggcgtgcaacaagaaggtgaccgaatcgctgatcaaggcgggtgcgttcgactcgctggggcatgcccgcaagggtcttttcctggtgcacagcgatgcggtggactcggtgctgggcaccaagaaggccgaggcactggggcagttcgatctcttcggcagcaatgatgatgggaccggcaccgcagatcccgtgttcaccatcaaggtgcccgatgatgagtgggaggacaaacacaaactcgccctagagcgcgagatgctgggactgtacgtctcggggcatcccctcaacggtgtggcacacttgctggctgcccaggtcgacaccgcgatcccagcgatcctcgacggcgatgtccccaacgatgcccaagtgcgggtgggcggcatcctggcgtcggtgaaccggagggtcaacaaaaacggaatgccatgggcttcagcgcaattggaggatctcacgggcggcatcgaggtgatgttcttcccgcacacctactccagctatggtgccgacatcgtcgacgatgccgtcgtgctggtcaacgccaaggtggcggtccgtgacgaccgcatcgcattgatcgccaatgacctcacagtgcccgacttttccaacgccgaggtggagcggccgctggcggtcagcttgcccacccggcagtgcacctttgacaaggtgagtgcgctcaaacaggtgttggcgcgccaccccggcacctcgcaggtgcatctgcggctcatca</t>
         </is>
       </c>
     </row>
@@ -866,12 +866,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>A491-S497_Block-2</t>
+          <t>T482-A484_Block-2</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>cgcctacgcgctgggcatcaccgacatcgacccgattccacacggtctgctgttcgagcggttcctcaaccccgagcgcacctcgatgcccgacatcgatatcgacttcgacgaccggcgccgcggtgagatggtgcgctacgcagccgacaagtggggccacgaccgggtcgcgcaggtcatcaccttcggcaccatcaaaaccaaagcggcgctgaaggattcggcgcgaatccactacgggcagcccgggttcgccatcgccgaccggatcaccaaggcgttgccgccggcgatcatgtctgggatcaccgatcccagccacgaacggtacaaggaggccgccgaggtccgcggcctgatcgaaaccgacccggacgtacgcaccatctaccagaccgcacgcgggttggaaggcctgatccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagcagcgagccgctgactgaggccatcccgttgtggaagcggccgcaggacggggccatcatcaccggctgggattacccggcgtgcgaggccatcggtc</t>
+          <t>gtactttctgatcgtcgccgacctgatcagctacgcgcggtcggcgggcataagggtgggtcccggccgcggctcggccgccggctcgctggtcgcctacgcgctgggcatcaccgacatcgacccgattccacacggtctgctgttcgagcggttcctcaaccccgagcgcacctcgatgcccgacatcgatatcgacttcgacgaccggcgccgcggtgagatggtgcgctacgcagccgacaagtggggccacgaccgggtcgcgcaggtcatcaccttcggcaccatcaaaaccaaagcggcgctgaaggattcggcgcgaatccactacgggcagcccgggttcgccatcgccgaccggatcgcgttgccgccggcgatcatggccaaagacatcccgctgtctgggatcaccgatcccagccacgaacggtacaaggaggccgccgaggtccgcggcctgatcgaaaccgacccggacgtacgcaccatctaccagaccgcacgcgggttggaaggcctgatccgcaacgcgggtgtgcacgcctgcgcggtgatcatgagcagcgagccgctgactgaggccatcccgttgtggaagcggccgcaggacggggccatcatcaccggctgggattacccggcgtgcgaggccatcggtctgctgaaaatggacttcctgggcctgcggaacctgacgatcatcggcgacgcgatcgacaacgtcagggccaacaggggtatcgacctcgacctggaatccgtgccgctggacgacaaggccacctatgagctgctgggccgcggcgacaccctgggcgtgttccagctcgacggcgggcccatgcgcgacctgctgcgccgcatgcagccgaccgggttcgaagacgtcgtcgccgttatcgcgctgtaccggcccggcccgatgggcatgaacgcacacaacgactatgccgaccgcaagaacaaccggcaggccatcaaacctattcacccggaactcgaag</t>
         </is>
       </c>
     </row>
@@ -883,12 +883,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>H127-K136_Block-0</t>
+          <t>R832-I836_Block-3</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>cggtgccagcgagttctacaactccgcgaccaaggccgggatcaagccgatcatcggcgtggaggcatacatcgcgccgggctcgcggttcgacacccggcgcatcctgtggggtgaccccagccaaaaggccgacgacgtctccggcagcggctcctacacgcacctgacgatgatggccgagaacgccaccggtctgcgcaacctgttcaagctgtcctcgaagtggtcgcgcatggacgccgagctcatcgccgaacacgccgagggcatcatcatcaccaccggatgcccgtcgggggaggtgcagacccgcctgcggctcggccaggatcgggaggcgctcgaagccgcggcgaagtggcgggagatcgtcggaccggacaactacttccttgagctgatggaccacgggctgaccatcgaacgccgggtccgtgacggtctgctcgagatcggacgcgcgctcaacattccgcctcttgccaccaatgactgccactacgtgacccgcgacgccgcccacaaccatgaggctt</t>
+          <t>cgacattctacgcaaggccatgggcaagaagaaacgcgaggtgctggagaaggagttcgagggcttctccgatggcatgcaggccaacgggttctctccggcggccatcaaggcgctgtgggacaccatcctgccgttcgctgactacgcgttcaacaagtcacatgccgccggctacggcatggtgtcctactggacggcctacctcaaggccaactatcccgccgagtacatggccggtctgttgacgtcggtcggcgacgataaagacaaggccgcggtttatctggccgactgcatcaccgtgctcccgcccgacgtcaacgaatctggcttgaacttcgcatcggtcggccaagacatccgctacgggctgggcgcggtgcgcaacgttggcgctaatgtcgtgggctcgttgctccaaacccgcaacgacaagggcaagttcaccgacttttcggactacctgaacaagatcgacatctcggcgtgcaacaagaaggtgaccgaatcgctgatcaaggcgggtgcgttcgactcgctggggcatgcccgcaagggtcttttcctggtgcacagcgatgcggtggactcggtgctgggcaccaagaaggccgaggcactggggcagttcgatctcttcggcagcaatgatgatgggaccggcaccgcagatcccgtgttcaccatcaaggtgcccgatgatgagtgggaggacaaacacaaactcgccctagagcgcgagatgctgggactgtacgtctcggggcatcccctcaacggtgtggcacacttgctggctgcccaggtcgacaccgcgatcccagcgatcctcgacggcgatgtccccaacgatgcccaagtgcgggtgggcggcatcctggcgtcggtgaaccggagggtcaacaaaaacggaatgccatgggcttcagcgcaattggaggatctcacgggcggcatcgaggtgatgttcttcccgcacacctactccagctatggtgccgacatcgtcgacgatgccgtcgtgctggtcaacgccaaggtggcggtccgtgacgaccgcatcgcattgatcgccaatgacctcacagtgcccgacttttccaacgccgaggtggagcggccgctggcggtcagcttgcccacccggcagtgcacctttgacaaggtgagtgcgctcaaacaggtgttggcgcgccaccccggcacctcgcaggtgcatctgcggctcatca</t>
         </is>
       </c>
     </row>

</xml_diff>